<commit_message>
working on writing results
</commit_message>
<xml_diff>
--- a/output/supplementary tables.xlsx
+++ b/output/supplementary tables.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmantegna/Documents/GitHub/WDFWmussels/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E63D18-846C-FF48-AECA-EA3378093EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F48409-F078-614A-AE80-999920BC1E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1540" windowWidth="27540" windowHeight="16940" activeTab="1" xr2:uid="{BE86B9F0-78FD-C044-9247-4161F6BEB5F3}"/>
+    <workbookView xWindow="31080" yWindow="2840" windowWidth="35600" windowHeight="16940" activeTab="4" xr2:uid="{BE86B9F0-78FD-C044-9247-4161F6BEB5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="analytes" sheetId="1" r:id="rId1"/>
     <sheet name="site-level data" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="kw pairwise comparisons" sheetId="3" r:id="rId3"/>
+    <sheet name="spearman &amp; kendalls corr" sheetId="4" r:id="rId4"/>
+    <sheet name="morans spatial autocorrelation" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="261">
   <si>
     <t>Class</t>
   </si>
@@ -455,13 +457,379 @@
   </si>
   <si>
     <t>ALL</t>
+  </si>
+  <si>
+    <t>reporting_area_1</t>
+  </si>
+  <si>
+    <t>reporting_area_2</t>
+  </si>
+  <si>
+    <t>p_value</t>
+  </si>
+  <si>
+    <t>group_1</t>
+  </si>
+  <si>
+    <t>group_2</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>KW + Dunns</t>
+  </si>
+  <si>
+    <t>Note - no SOD significant results</t>
+  </si>
+  <si>
+    <t>Condition Index 1</t>
+  </si>
+  <si>
+    <t>site_1</t>
+  </si>
+  <si>
+    <t>site_2</t>
+  </si>
+  <si>
+    <t>Eagle Harbor Dr</t>
+  </si>
+  <si>
+    <t>Lions Park</t>
+  </si>
+  <si>
+    <t>Edmonds Ferry</t>
+  </si>
+  <si>
+    <t>IBR biomarkers</t>
+  </si>
+  <si>
+    <t>IBR morphology</t>
+  </si>
+  <si>
+    <t>Eastsound, Fishing Bay</t>
+  </si>
+  <si>
+    <t>Chambers Bay Park</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Suquamish, Stormwater Outfall</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>Des Moines Marina</t>
+  </si>
+  <si>
+    <t>ade</t>
+  </si>
+  <si>
+    <t>Jamestown</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>Gig Harbor Boat Launch</t>
+  </si>
+  <si>
+    <t>abde</t>
+  </si>
+  <si>
+    <t>Shilshole Bay</t>
+  </si>
+  <si>
+    <t>Skiff Point</t>
+  </si>
+  <si>
+    <t>Thea Foss Waterway</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>Minter Bay</t>
+  </si>
+  <si>
+    <t>Penn Cove Reference</t>
+  </si>
+  <si>
+    <t>cfg</t>
+  </si>
+  <si>
+    <t>Manchester, Stormwater Outfall</t>
+  </si>
+  <si>
+    <t>Purdy, Burley Lagoon</t>
+  </si>
+  <si>
+    <t>Tulalip Bay</t>
+  </si>
+  <si>
+    <t>Arroyo Beach</t>
+  </si>
+  <si>
+    <t>Chimacum Creek delta</t>
+  </si>
+  <si>
+    <t>Hood Canal Holly</t>
+  </si>
+  <si>
+    <t>bcfg</t>
+  </si>
+  <si>
+    <t>Cherry Point Aquatic Reserve, Conoco Phillips</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>Raft Island Park</t>
+  </si>
+  <si>
+    <t>Broad Spit</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>Salmon Beach</t>
+  </si>
+  <si>
+    <t>Blair Waterway Two</t>
+  </si>
+  <si>
+    <t>Penrose Point State Park</t>
+  </si>
+  <si>
+    <t>Filucy Bay</t>
+  </si>
+  <si>
+    <t>Squaxin Island</t>
+  </si>
+  <si>
+    <t>Elliott Bay, Harbor Island, Pier 17</t>
+  </si>
+  <si>
+    <t>Maristone Island</t>
+  </si>
+  <si>
+    <t>abcfg</t>
+  </si>
+  <si>
+    <t>Williams Olson Park</t>
+  </si>
+  <si>
+    <t>Brackenwood Lane</t>
+  </si>
+  <si>
+    <t>Browns Point Lighthouse</t>
+  </si>
+  <si>
+    <t>Purdy, Dexters</t>
+  </si>
+  <si>
+    <t>Elliot Bay Myrtle Edwards</t>
+  </si>
+  <si>
+    <t>Seattle Aquarium, Pier 59</t>
+  </si>
+  <si>
+    <t>Commencement Bay, Milwaukee Waterway</t>
+  </si>
+  <si>
+    <t>Blair Waterway</t>
+  </si>
+  <si>
+    <t>Point Defiance Ferry</t>
+  </si>
+  <si>
+    <t>Locust Beach</t>
+  </si>
+  <si>
+    <t>Silverdale, Dyes Inlet</t>
+  </si>
+  <si>
+    <t>Port Angeles Yacht Club</t>
+  </si>
+  <si>
+    <t>Kitsap St Boat Launch</t>
+  </si>
+  <si>
+    <t>Commencement Bay, Dick Gilmur Launch</t>
+  </si>
+  <si>
+    <t>Rocky Point</t>
+  </si>
+  <si>
+    <t>N Avenue Park</t>
+  </si>
+  <si>
+    <t>Miller Creek</t>
+  </si>
+  <si>
+    <t>Eld Inlet</t>
+  </si>
+  <si>
+    <t>abcefg</t>
+  </si>
+  <si>
+    <t>Salmon Bay, Commodore Park</t>
+  </si>
+  <si>
+    <t>Three Tree Point</t>
+  </si>
+  <si>
+    <t>Aiston Preserve</t>
+  </si>
+  <si>
+    <t>Kingston Marina</t>
+  </si>
+  <si>
+    <t>Rich Passage</t>
+  </si>
+  <si>
+    <t>Madrona Pont</t>
+  </si>
+  <si>
+    <t>Discovery Bay</t>
+  </si>
+  <si>
+    <t>Chuckanut, Clark's Point</t>
+  </si>
+  <si>
+    <t>Mukilteo</t>
+  </si>
+  <si>
+    <t>IBR combined</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOVA + Tukeys </t>
+  </si>
+  <si>
+    <t>ANOVA + Tukeys</t>
+  </si>
+  <si>
+    <t>geo_cluster_1</t>
+  </si>
+  <si>
+    <t>geo_cluster_2</t>
+  </si>
+  <si>
+    <t>Global Moran's I Summary</t>
+  </si>
+  <si>
+    <t>Analyte Class</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>moran_i</t>
+  </si>
+  <si>
+    <t>expected_i</t>
+  </si>
+  <si>
+    <t>chlordane</t>
+  </si>
+  <si>
+    <t>ddt</t>
+  </si>
+  <si>
+    <t>hch</t>
+  </si>
+  <si>
+    <t>hmw</t>
+  </si>
+  <si>
+    <t>lmw</t>
+  </si>
+  <si>
+    <t>pbde</t>
+  </si>
+  <si>
+    <t>pbde_congener</t>
+  </si>
+  <si>
+    <t>pcb</t>
+  </si>
+  <si>
+    <t>pesticide</t>
+  </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>ibr1overall</t>
+  </si>
+  <si>
+    <t>ibr1bio</t>
+  </si>
+  <si>
+    <t>p450</t>
+  </si>
+  <si>
+    <t>ibr1morph</t>
+  </si>
+  <si>
+    <t>shell</t>
+  </si>
+  <si>
+    <t>ci1</t>
+  </si>
+  <si>
+    <t>ci2</t>
+  </si>
+  <si>
+    <t>ci3</t>
+  </si>
+  <si>
+    <t>sod</t>
+  </si>
+  <si>
+    <t>Metals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mercury </t>
+  </si>
+  <si>
+    <t>corr_long</t>
+  </si>
+  <si>
+    <t>Note the longitudinal correlation versus global corr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -481,6 +849,20 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -516,11 +898,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,7 +1819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC38454-BABA-6748-BCE4-7657067C7BC4}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1529,6 +1919,2836 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1164540B-E78A-5C4C-B904-DC87BC623030}">
+  <dimension ref="A1:AC107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="2.1640625" customWidth="1"/>
+    <col min="12" max="12" width="1.83203125" customWidth="1"/>
+    <col min="18" max="18" width="2" customWidth="1"/>
+    <col min="24" max="24" width="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" t="s">
+        <v>148</v>
+      </c>
+      <c r="S1" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="Y2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4">
+        <v>3.1800000000000002E-2</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S4" t="s">
+        <v>158</v>
+      </c>
+      <c r="T4" t="s">
+        <v>159</v>
+      </c>
+      <c r="U4" s="4">
+        <v>1.11170284089468E-9</v>
+      </c>
+      <c r="V4" t="s">
+        <v>160</v>
+      </c>
+      <c r="W4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1.08759E-3</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="O5">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>146</v>
+      </c>
+      <c r="S5" t="s">
+        <v>162</v>
+      </c>
+      <c r="T5" t="s">
+        <v>158</v>
+      </c>
+      <c r="U5" s="4">
+        <v>1.8098114451525799E-8</v>
+      </c>
+      <c r="V5" t="s">
+        <v>163</v>
+      </c>
+      <c r="W5" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>12</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>11</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>3.3052799999999999E-3</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="M6">
+        <v>11</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+      <c r="O6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6" t="s">
+        <v>158</v>
+      </c>
+      <c r="T6" t="s">
+        <v>164</v>
+      </c>
+      <c r="U6" s="4">
+        <v>1.3669200882304701E-7</v>
+      </c>
+      <c r="V6" t="s">
+        <v>160</v>
+      </c>
+      <c r="W6" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>3.79701E-3</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="s">
+        <v>145</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>13</v>
+      </c>
+      <c r="O7">
+        <v>1.67E-2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" t="s">
+        <v>166</v>
+      </c>
+      <c r="T7" t="s">
+        <v>159</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1.4735145625888201E-7</v>
+      </c>
+      <c r="V7" t="s">
+        <v>167</v>
+      </c>
+      <c r="W7" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>9.0221999999999993E-3</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>147</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>12</v>
+      </c>
+      <c r="O8">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>144</v>
+      </c>
+      <c r="S8" t="s">
+        <v>168</v>
+      </c>
+      <c r="T8" t="s">
+        <v>158</v>
+      </c>
+      <c r="U8" s="4">
+        <v>1.27025597673747E-6</v>
+      </c>
+      <c r="V8" t="s">
+        <v>169</v>
+      </c>
+      <c r="W8" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>12</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>2.7012109999999999E-2</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C9">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9">
+        <v>12</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="P9" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>147</v>
+      </c>
+      <c r="S9" t="s">
+        <v>170</v>
+      </c>
+      <c r="T9" t="s">
+        <v>159</v>
+      </c>
+      <c r="U9" s="4">
+        <v>1.2702559769595099E-6</v>
+      </c>
+      <c r="V9" t="s">
+        <v>167</v>
+      </c>
+      <c r="W9" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>3.3340689999999999E-2</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" t="s">
+        <v>146</v>
+      </c>
+      <c r="M10">
+        <v>13</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <v>2.92E-2</v>
+      </c>
+      <c r="P10" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>147</v>
+      </c>
+      <c r="S10" t="s">
+        <v>171</v>
+      </c>
+      <c r="T10" t="s">
+        <v>159</v>
+      </c>
+      <c r="U10" s="4">
+        <v>1.5231958298000901E-6</v>
+      </c>
+      <c r="V10" t="s">
+        <v>167</v>
+      </c>
+      <c r="W10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" t="s">
+        <v>144</v>
+      </c>
+      <c r="M11">
+        <v>12</v>
+      </c>
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>2.9899999999999999E-2</v>
+      </c>
+      <c r="P11" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>146</v>
+      </c>
+      <c r="S11" t="s">
+        <v>162</v>
+      </c>
+      <c r="T11" t="s">
+        <v>166</v>
+      </c>
+      <c r="U11" s="4">
+        <v>2.4933619541256399E-6</v>
+      </c>
+      <c r="V11" t="s">
+        <v>163</v>
+      </c>
+      <c r="W11" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z11" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA11" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC11" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>4.02E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12">
+        <v>6</v>
+      </c>
+      <c r="O12">
+        <v>3.7400000000000003E-2</v>
+      </c>
+      <c r="P12" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>146</v>
+      </c>
+      <c r="S12" t="s">
+        <v>162</v>
+      </c>
+      <c r="T12" t="s">
+        <v>170</v>
+      </c>
+      <c r="U12" s="4">
+        <v>1.51575491591505E-5</v>
+      </c>
+      <c r="V12" t="s">
+        <v>163</v>
+      </c>
+      <c r="W12" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y12">
+        <v>4</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>5.6344151406762E-6</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>146</v>
+      </c>
+      <c r="S13" t="s">
+        <v>162</v>
+      </c>
+      <c r="T13" t="s">
+        <v>171</v>
+      </c>
+      <c r="U13" s="4">
+        <v>1.7996393042785101E-5</v>
+      </c>
+      <c r="V13" t="s">
+        <v>163</v>
+      </c>
+      <c r="W13" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y13">
+        <v>5</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>9.2330487887703997E-5</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C14">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S14" t="s">
+        <v>166</v>
+      </c>
+      <c r="T14" t="s">
+        <v>164</v>
+      </c>
+      <c r="U14" s="4">
+        <v>1.87349634145351E-5</v>
+      </c>
+      <c r="V14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y14">
+        <v>6</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1.9981706250138401E-4</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>1.26E-2</v>
+      </c>
+      <c r="P15" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>144</v>
+      </c>
+      <c r="S15" t="s">
+        <v>172</v>
+      </c>
+      <c r="T15" t="s">
+        <v>158</v>
+      </c>
+      <c r="U15" s="4">
+        <v>2.92453696609796E-5</v>
+      </c>
+      <c r="V15" t="s">
+        <v>173</v>
+      </c>
+      <c r="W15" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y15">
+        <v>2</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>1.06200416421028E-2</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>144</v>
+      </c>
+      <c r="S16" t="s">
+        <v>174</v>
+      </c>
+      <c r="T16" t="s">
+        <v>158</v>
+      </c>
+      <c r="U16" s="4">
+        <v>3.5487911469234101E-5</v>
+      </c>
+      <c r="V16" t="s">
+        <v>173</v>
+      </c>
+      <c r="W16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="P17" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>144</v>
+      </c>
+      <c r="S17" t="s">
+        <v>175</v>
+      </c>
+      <c r="T17" t="s">
+        <v>159</v>
+      </c>
+      <c r="U17" s="4">
+        <v>4.1971514050498398E-5</v>
+      </c>
+      <c r="V17" t="s">
+        <v>176</v>
+      </c>
+      <c r="W17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" t="s">
+        <v>226</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>3.09E-2</v>
+      </c>
+      <c r="P18" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>226</v>
+      </c>
+      <c r="S18" t="s">
+        <v>177</v>
+      </c>
+      <c r="T18" t="s">
+        <v>159</v>
+      </c>
+      <c r="U18" s="4">
+        <v>4.1971514050720402E-5</v>
+      </c>
+      <c r="V18" t="s">
+        <v>176</v>
+      </c>
+      <c r="W18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" t="s">
+        <v>144</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>6</v>
+      </c>
+      <c r="O19">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="P19" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>226</v>
+      </c>
+      <c r="S19" t="s">
+        <v>178</v>
+      </c>
+      <c r="T19" t="s">
+        <v>158</v>
+      </c>
+      <c r="U19" s="4">
+        <v>4.1971514178063003E-5</v>
+      </c>
+      <c r="V19" t="s">
+        <v>173</v>
+      </c>
+      <c r="W19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" t="s">
+        <v>226</v>
+      </c>
+      <c r="S20" t="s">
+        <v>179</v>
+      </c>
+      <c r="T20" t="s">
+        <v>158</v>
+      </c>
+      <c r="U20" s="4">
+        <v>4.72760023618735E-5</v>
+      </c>
+      <c r="V20" t="s">
+        <v>173</v>
+      </c>
+      <c r="W20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1.34E-2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>144</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="S21" t="s">
+        <v>158</v>
+      </c>
+      <c r="T21" t="s">
+        <v>180</v>
+      </c>
+      <c r="U21" s="4">
+        <v>6.4023026579040896E-5</v>
+      </c>
+      <c r="V21" t="s">
+        <v>160</v>
+      </c>
+      <c r="W21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" t="s">
+        <v>226</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S22" t="s">
+        <v>170</v>
+      </c>
+      <c r="T22" t="s">
+        <v>164</v>
+      </c>
+      <c r="U22" s="4">
+        <v>8.8418687683500306E-5</v>
+      </c>
+      <c r="V22" t="s">
+        <v>167</v>
+      </c>
+      <c r="W22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" t="s">
+        <v>226</v>
+      </c>
+      <c r="M23">
+        <v>11</v>
+      </c>
+      <c r="N23">
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>145</v>
+      </c>
+      <c r="S23" t="s">
+        <v>158</v>
+      </c>
+      <c r="T23" t="s">
+        <v>181</v>
+      </c>
+      <c r="U23" s="4">
+        <v>8.8418688075964105E-5</v>
+      </c>
+      <c r="V23" t="s">
+        <v>160</v>
+      </c>
+      <c r="W23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>13</v>
+      </c>
+      <c r="N24">
+        <v>7</v>
+      </c>
+      <c r="O24">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="P24" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>145</v>
+      </c>
+      <c r="S24" t="s">
+        <v>171</v>
+      </c>
+      <c r="T24" t="s">
+        <v>164</v>
+      </c>
+      <c r="U24">
+        <v>1.04103425343727E-4</v>
+      </c>
+      <c r="V24" t="s">
+        <v>167</v>
+      </c>
+      <c r="W24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="S25" t="s">
+        <v>166</v>
+      </c>
+      <c r="T25" t="s">
+        <v>168</v>
+      </c>
+      <c r="U25">
+        <v>1.65831566107499E-4</v>
+      </c>
+      <c r="V25" t="s">
+        <v>167</v>
+      </c>
+      <c r="W25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M26" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q26" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S26" t="s">
+        <v>158</v>
+      </c>
+      <c r="T26" t="s">
+        <v>153</v>
+      </c>
+      <c r="U26">
+        <v>1.83132698287181E-4</v>
+      </c>
+      <c r="V26" t="s">
+        <v>160</v>
+      </c>
+      <c r="W26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>6</v>
+      </c>
+      <c r="O27">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="P27" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>145</v>
+      </c>
+      <c r="S27" t="s">
+        <v>182</v>
+      </c>
+      <c r="T27" t="s">
+        <v>159</v>
+      </c>
+      <c r="U27">
+        <v>3.8288649192885798E-4</v>
+      </c>
+      <c r="V27" t="s">
+        <v>183</v>
+      </c>
+      <c r="W27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>6</v>
+      </c>
+      <c r="O28">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="P28" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>145</v>
+      </c>
+      <c r="S28" t="s">
+        <v>162</v>
+      </c>
+      <c r="T28" t="s">
+        <v>175</v>
+      </c>
+      <c r="U28">
+        <v>4.02736125371006E-4</v>
+      </c>
+      <c r="V28" t="s">
+        <v>163</v>
+      </c>
+      <c r="W28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="N29">
+        <v>6</v>
+      </c>
+      <c r="O29">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="P29" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>145</v>
+      </c>
+      <c r="S29" t="s">
+        <v>162</v>
+      </c>
+      <c r="T29" t="s">
+        <v>177</v>
+      </c>
+      <c r="U29">
+        <v>4.0273612537111703E-4</v>
+      </c>
+      <c r="V29" t="s">
+        <v>163</v>
+      </c>
+      <c r="W29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="S30" t="s">
+        <v>170</v>
+      </c>
+      <c r="T30" t="s">
+        <v>168</v>
+      </c>
+      <c r="U30">
+        <v>5.9208322503467902E-4</v>
+      </c>
+      <c r="V30" t="s">
+        <v>167</v>
+      </c>
+      <c r="W30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M31" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="S31" t="s">
+        <v>171</v>
+      </c>
+      <c r="T31" t="s">
+        <v>168</v>
+      </c>
+      <c r="U31">
+        <v>6.8960471787038501E-4</v>
+      </c>
+      <c r="V31" t="s">
+        <v>167</v>
+      </c>
+      <c r="W31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="M32" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S32" t="s">
+        <v>158</v>
+      </c>
+      <c r="T32" t="s">
+        <v>184</v>
+      </c>
+      <c r="U32">
+        <v>8.0240597463954199E-4</v>
+      </c>
+      <c r="V32" t="s">
+        <v>160</v>
+      </c>
+      <c r="W32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>13</v>
+      </c>
+      <c r="N33">
+        <v>7</v>
+      </c>
+      <c r="O33">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="P33" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>145</v>
+      </c>
+      <c r="S33" t="s">
+        <v>186</v>
+      </c>
+      <c r="T33" t="s">
+        <v>159</v>
+      </c>
+      <c r="U33">
+        <v>8.6522806239064398E-4</v>
+      </c>
+      <c r="V33" t="s">
+        <v>183</v>
+      </c>
+      <c r="W33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>11</v>
+      </c>
+      <c r="N34">
+        <v>7</v>
+      </c>
+      <c r="O34">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="P34" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>145</v>
+      </c>
+      <c r="S34" t="s">
+        <v>159</v>
+      </c>
+      <c r="T34" t="s">
+        <v>187</v>
+      </c>
+      <c r="U34">
+        <v>8.7328633276906298E-4</v>
+      </c>
+      <c r="V34" t="s">
+        <v>161</v>
+      </c>
+      <c r="W34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S35" t="s">
+        <v>189</v>
+      </c>
+      <c r="T35" t="s">
+        <v>158</v>
+      </c>
+      <c r="U35">
+        <v>1.0831522205368999E-3</v>
+      </c>
+      <c r="V35" t="s">
+        <v>185</v>
+      </c>
+      <c r="W35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M36" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="S36" t="s">
+        <v>158</v>
+      </c>
+      <c r="T36" t="s">
+        <v>190</v>
+      </c>
+      <c r="U36">
+        <v>1.56702634865014E-3</v>
+      </c>
+      <c r="V36" t="s">
+        <v>160</v>
+      </c>
+      <c r="W36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37">
+        <v>6</v>
+      </c>
+      <c r="O37">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="P37" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>145</v>
+      </c>
+      <c r="S37" t="s">
+        <v>191</v>
+      </c>
+      <c r="T37" t="s">
+        <v>158</v>
+      </c>
+      <c r="U37">
+        <v>1.56702634968864E-3</v>
+      </c>
+      <c r="V37" t="s">
+        <v>185</v>
+      </c>
+      <c r="W37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>6</v>
+      </c>
+      <c r="O38">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P38" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>145</v>
+      </c>
+      <c r="S38" t="s">
+        <v>192</v>
+      </c>
+      <c r="T38" t="s">
+        <v>158</v>
+      </c>
+      <c r="U38">
+        <v>1.68583571024561E-3</v>
+      </c>
+      <c r="V38" t="s">
+        <v>185</v>
+      </c>
+      <c r="W38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="S39" t="s">
+        <v>193</v>
+      </c>
+      <c r="T39" t="s">
+        <v>158</v>
+      </c>
+      <c r="U39">
+        <v>1.6858357113544999E-3</v>
+      </c>
+      <c r="V39" t="s">
+        <v>185</v>
+      </c>
+      <c r="W39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S40" t="s">
+        <v>194</v>
+      </c>
+      <c r="T40" t="s">
+        <v>158</v>
+      </c>
+      <c r="U40">
+        <v>1.6858357124656101E-3</v>
+      </c>
+      <c r="V40" t="s">
+        <v>185</v>
+      </c>
+      <c r="W40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S41" t="s">
+        <v>195</v>
+      </c>
+      <c r="T41" t="s">
+        <v>159</v>
+      </c>
+      <c r="U41">
+        <v>1.69419911751811E-3</v>
+      </c>
+      <c r="V41" t="s">
+        <v>196</v>
+      </c>
+      <c r="W41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S42" t="s">
+        <v>177</v>
+      </c>
+      <c r="T42" t="s">
+        <v>164</v>
+      </c>
+      <c r="U42">
+        <v>1.9496136349282901E-3</v>
+      </c>
+      <c r="V42" t="s">
+        <v>176</v>
+      </c>
+      <c r="W42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S43" t="s">
+        <v>175</v>
+      </c>
+      <c r="T43" t="s">
+        <v>164</v>
+      </c>
+      <c r="U43">
+        <v>1.9496136349296299E-3</v>
+      </c>
+      <c r="V43" t="s">
+        <v>176</v>
+      </c>
+      <c r="W43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S44" t="s">
+        <v>197</v>
+      </c>
+      <c r="T44" t="s">
+        <v>159</v>
+      </c>
+      <c r="U44">
+        <v>2.4197750131560399E-3</v>
+      </c>
+      <c r="V44" t="s">
+        <v>196</v>
+      </c>
+      <c r="W44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S45" t="s">
+        <v>159</v>
+      </c>
+      <c r="T45" t="s">
+        <v>198</v>
+      </c>
+      <c r="U45">
+        <v>2.41977501315738E-3</v>
+      </c>
+      <c r="V45" t="s">
+        <v>161</v>
+      </c>
+      <c r="W45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S46" t="s">
+        <v>158</v>
+      </c>
+      <c r="T46" t="s">
+        <v>199</v>
+      </c>
+      <c r="U46">
+        <v>2.59904762547436E-3</v>
+      </c>
+      <c r="V46" t="s">
+        <v>160</v>
+      </c>
+      <c r="W46" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S47" t="s">
+        <v>200</v>
+      </c>
+      <c r="T47" t="s">
+        <v>158</v>
+      </c>
+      <c r="U47">
+        <v>3.4495893648821599E-3</v>
+      </c>
+      <c r="V47" t="s">
+        <v>185</v>
+      </c>
+      <c r="W47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="S48" t="s">
+        <v>201</v>
+      </c>
+      <c r="T48" t="s">
+        <v>158</v>
+      </c>
+      <c r="U48">
+        <v>3.51424901660913E-3</v>
+      </c>
+      <c r="V48" t="s">
+        <v>185</v>
+      </c>
+      <c r="W48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S49" t="s">
+        <v>172</v>
+      </c>
+      <c r="T49" t="s">
+        <v>166</v>
+      </c>
+      <c r="U49">
+        <v>3.6056641560834302E-3</v>
+      </c>
+      <c r="V49" t="s">
+        <v>173</v>
+      </c>
+      <c r="W49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S50" t="s">
+        <v>202</v>
+      </c>
+      <c r="T50" t="s">
+        <v>158</v>
+      </c>
+      <c r="U50">
+        <v>3.6999882041188802E-3</v>
+      </c>
+      <c r="V50" t="s">
+        <v>185</v>
+      </c>
+      <c r="W50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S51" t="s">
+        <v>162</v>
+      </c>
+      <c r="T51" t="s">
+        <v>182</v>
+      </c>
+      <c r="U51">
+        <v>3.70576165320902E-3</v>
+      </c>
+      <c r="V51" t="s">
+        <v>163</v>
+      </c>
+      <c r="W51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S52" t="s">
+        <v>174</v>
+      </c>
+      <c r="T52" t="s">
+        <v>166</v>
+      </c>
+      <c r="U52">
+        <v>3.8015277646730201E-3</v>
+      </c>
+      <c r="V52" t="s">
+        <v>173</v>
+      </c>
+      <c r="W52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S53" t="s">
+        <v>158</v>
+      </c>
+      <c r="T53" t="s">
+        <v>203</v>
+      </c>
+      <c r="U53">
+        <v>4.1927511450138297E-3</v>
+      </c>
+      <c r="V53" t="s">
+        <v>160</v>
+      </c>
+      <c r="W53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S54" t="s">
+        <v>178</v>
+      </c>
+      <c r="T54" t="s">
+        <v>166</v>
+      </c>
+      <c r="U54">
+        <v>4.4268281728420096E-3</v>
+      </c>
+      <c r="V54" t="s">
+        <v>173</v>
+      </c>
+      <c r="W54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S55" t="s">
+        <v>158</v>
+      </c>
+      <c r="T55" t="s">
+        <v>204</v>
+      </c>
+      <c r="U55">
+        <v>4.5577636859716001E-3</v>
+      </c>
+      <c r="V55" t="s">
+        <v>160</v>
+      </c>
+      <c r="W55" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S56" t="s">
+        <v>205</v>
+      </c>
+      <c r="T56" t="s">
+        <v>158</v>
+      </c>
+      <c r="U56">
+        <v>4.5577636916573896E-3</v>
+      </c>
+      <c r="V56" t="s">
+        <v>185</v>
+      </c>
+      <c r="W56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S57" t="s">
+        <v>162</v>
+      </c>
+      <c r="T57" t="s">
+        <v>187</v>
+      </c>
+      <c r="U57">
+        <v>5.61732492768241E-3</v>
+      </c>
+      <c r="V57" t="s">
+        <v>163</v>
+      </c>
+      <c r="W57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S58" t="s">
+        <v>206</v>
+      </c>
+      <c r="T58" t="s">
+        <v>159</v>
+      </c>
+      <c r="U58">
+        <v>5.9938782066703E-3</v>
+      </c>
+      <c r="V58" t="s">
+        <v>196</v>
+      </c>
+      <c r="W58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S59" t="s">
+        <v>207</v>
+      </c>
+      <c r="T59" t="s">
+        <v>159</v>
+      </c>
+      <c r="U59">
+        <v>5.9938782103459197E-3</v>
+      </c>
+      <c r="V59" t="s">
+        <v>196</v>
+      </c>
+      <c r="W59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S60" t="s">
+        <v>179</v>
+      </c>
+      <c r="T60" t="s">
+        <v>166</v>
+      </c>
+      <c r="U60">
+        <v>6.0942299975218503E-3</v>
+      </c>
+      <c r="V60" t="s">
+        <v>173</v>
+      </c>
+      <c r="W60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S61" t="s">
+        <v>208</v>
+      </c>
+      <c r="T61" t="s">
+        <v>158</v>
+      </c>
+      <c r="U61">
+        <v>6.2810215492624701E-3</v>
+      </c>
+      <c r="V61" t="s">
+        <v>185</v>
+      </c>
+      <c r="W61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S62" t="s">
+        <v>209</v>
+      </c>
+      <c r="T62" t="s">
+        <v>158</v>
+      </c>
+      <c r="U62">
+        <v>6.4139077573951396E-3</v>
+      </c>
+      <c r="V62" t="s">
+        <v>185</v>
+      </c>
+      <c r="W62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S63" t="s">
+        <v>158</v>
+      </c>
+      <c r="T63" t="s">
+        <v>210</v>
+      </c>
+      <c r="U63">
+        <v>6.4139077573956999E-3</v>
+      </c>
+      <c r="V63" t="s">
+        <v>160</v>
+      </c>
+      <c r="W63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S64" t="s">
+        <v>211</v>
+      </c>
+      <c r="T64" t="s">
+        <v>159</v>
+      </c>
+      <c r="U64">
+        <v>6.4139077613091199E-3</v>
+      </c>
+      <c r="V64" t="s">
+        <v>196</v>
+      </c>
+      <c r="W64" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S65" t="s">
+        <v>162</v>
+      </c>
+      <c r="T65" t="s">
+        <v>186</v>
+      </c>
+      <c r="U65">
+        <v>6.41390776914408E-3</v>
+      </c>
+      <c r="V65" t="s">
+        <v>163</v>
+      </c>
+      <c r="W65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S66" t="s">
+        <v>155</v>
+      </c>
+      <c r="T66" t="s">
+        <v>159</v>
+      </c>
+      <c r="U66">
+        <v>6.8612902456063303E-3</v>
+      </c>
+      <c r="V66" t="s">
+        <v>196</v>
+      </c>
+      <c r="W66" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S67" t="s">
+        <v>166</v>
+      </c>
+      <c r="T67" t="s">
+        <v>180</v>
+      </c>
+      <c r="U67">
+        <v>8.0174843222197093E-3</v>
+      </c>
+      <c r="V67" t="s">
+        <v>167</v>
+      </c>
+      <c r="W67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S68" t="s">
+        <v>166</v>
+      </c>
+      <c r="T68" t="s">
+        <v>181</v>
+      </c>
+      <c r="U68">
+        <v>8.6306354695675509E-3</v>
+      </c>
+      <c r="V68" t="s">
+        <v>167</v>
+      </c>
+      <c r="W68" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="69" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S69" t="s">
+        <v>170</v>
+      </c>
+      <c r="T69" t="s">
+        <v>174</v>
+      </c>
+      <c r="U69">
+        <v>8.9577718896062305E-3</v>
+      </c>
+      <c r="V69" t="s">
+        <v>167</v>
+      </c>
+      <c r="W69" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S70" t="s">
+        <v>172</v>
+      </c>
+      <c r="T70" t="s">
+        <v>170</v>
+      </c>
+      <c r="U70">
+        <v>9.9874485832181E-3</v>
+      </c>
+      <c r="V70" t="s">
+        <v>173</v>
+      </c>
+      <c r="W70" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S71" t="s">
+        <v>175</v>
+      </c>
+      <c r="T71" t="s">
+        <v>168</v>
+      </c>
+      <c r="U71">
+        <v>1.02159582639959E-2</v>
+      </c>
+      <c r="V71" t="s">
+        <v>176</v>
+      </c>
+      <c r="W71" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S72" t="s">
+        <v>177</v>
+      </c>
+      <c r="T72" t="s">
+        <v>168</v>
+      </c>
+      <c r="U72">
+        <v>1.0215958263995999E-2</v>
+      </c>
+      <c r="V72" t="s">
+        <v>176</v>
+      </c>
+      <c r="W72" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S73" t="s">
+        <v>171</v>
+      </c>
+      <c r="T73" t="s">
+        <v>174</v>
+      </c>
+      <c r="U73">
+        <v>1.02159582700281E-2</v>
+      </c>
+      <c r="V73" t="s">
+        <v>167</v>
+      </c>
+      <c r="W73" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S74" t="s">
+        <v>170</v>
+      </c>
+      <c r="T74" t="s">
+        <v>178</v>
+      </c>
+      <c r="U74">
+        <v>1.0215958300202501E-2</v>
+      </c>
+      <c r="V74" t="s">
+        <v>167</v>
+      </c>
+      <c r="W74" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S75" t="s">
+        <v>212</v>
+      </c>
+      <c r="T75" t="s">
+        <v>158</v>
+      </c>
+      <c r="U75">
+        <v>1.09046134067058E-2</v>
+      </c>
+      <c r="V75" t="s">
+        <v>185</v>
+      </c>
+      <c r="W75" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S76" t="s">
+        <v>172</v>
+      </c>
+      <c r="T76" t="s">
+        <v>171</v>
+      </c>
+      <c r="U76">
+        <v>1.1458295439051899E-2</v>
+      </c>
+      <c r="V76" t="s">
+        <v>173</v>
+      </c>
+      <c r="W76" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S77" t="s">
+        <v>213</v>
+      </c>
+      <c r="T77" t="s">
+        <v>158</v>
+      </c>
+      <c r="U77">
+        <v>1.1635926752725401E-2</v>
+      </c>
+      <c r="V77" t="s">
+        <v>185</v>
+      </c>
+      <c r="W77" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S78" t="s">
+        <v>171</v>
+      </c>
+      <c r="T78" t="s">
+        <v>178</v>
+      </c>
+      <c r="U78">
+        <v>1.16359267731418E-2</v>
+      </c>
+      <c r="V78" t="s">
+        <v>167</v>
+      </c>
+      <c r="W78" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S79" t="s">
+        <v>162</v>
+      </c>
+      <c r="T79" t="s">
+        <v>195</v>
+      </c>
+      <c r="U79">
+        <v>1.3877872065973899E-2</v>
+      </c>
+      <c r="V79" t="s">
+        <v>163</v>
+      </c>
+      <c r="W79" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="80" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S80" t="s">
+        <v>162</v>
+      </c>
+      <c r="T80" t="s">
+        <v>198</v>
+      </c>
+      <c r="U80">
+        <v>1.60179211041763E-2</v>
+      </c>
+      <c r="V80" t="s">
+        <v>163</v>
+      </c>
+      <c r="W80" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S81" t="s">
+        <v>197</v>
+      </c>
+      <c r="T81" t="s">
+        <v>162</v>
+      </c>
+      <c r="U81">
+        <v>1.60179211041773E-2</v>
+      </c>
+      <c r="V81" t="s">
+        <v>196</v>
+      </c>
+      <c r="W81" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S82" t="s">
+        <v>166</v>
+      </c>
+      <c r="T82" t="s">
+        <v>153</v>
+      </c>
+      <c r="U82">
+        <v>1.63199435226308E-2</v>
+      </c>
+      <c r="V82" t="s">
+        <v>167</v>
+      </c>
+      <c r="W82" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S83" t="s">
+        <v>214</v>
+      </c>
+      <c r="T83" t="s">
+        <v>159</v>
+      </c>
+      <c r="U83">
+        <v>1.7058033441290199E-2</v>
+      </c>
+      <c r="V83" t="s">
+        <v>215</v>
+      </c>
+      <c r="W83" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S84" t="s">
+        <v>216</v>
+      </c>
+      <c r="T84" t="s">
+        <v>159</v>
+      </c>
+      <c r="U84">
+        <v>1.7058033441293401E-2</v>
+      </c>
+      <c r="V84" t="s">
+        <v>215</v>
+      </c>
+      <c r="W84" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S85" t="s">
+        <v>182</v>
+      </c>
+      <c r="T85" t="s">
+        <v>164</v>
+      </c>
+      <c r="U85">
+        <v>1.7086571105509301E-2</v>
+      </c>
+      <c r="V85" t="s">
+        <v>183</v>
+      </c>
+      <c r="W85" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S86" t="s">
+        <v>179</v>
+      </c>
+      <c r="T86" t="s">
+        <v>170</v>
+      </c>
+      <c r="U86">
+        <v>1.74820869320499E-2</v>
+      </c>
+      <c r="V86" t="s">
+        <v>173</v>
+      </c>
+      <c r="W86" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S87" t="s">
+        <v>170</v>
+      </c>
+      <c r="T87" t="s">
+        <v>181</v>
+      </c>
+      <c r="U87">
+        <v>1.8159452973116399E-2</v>
+      </c>
+      <c r="V87" t="s">
+        <v>167</v>
+      </c>
+      <c r="W87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S88" t="s">
+        <v>217</v>
+      </c>
+      <c r="T88" t="s">
+        <v>158</v>
+      </c>
+      <c r="U88">
+        <v>1.8159452993586699E-2</v>
+      </c>
+      <c r="V88" t="s">
+        <v>185</v>
+      </c>
+      <c r="W88" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="89" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S89" t="s">
+        <v>158</v>
+      </c>
+      <c r="T89" t="s">
+        <v>218</v>
+      </c>
+      <c r="U89">
+        <v>1.9325300460549599E-2</v>
+      </c>
+      <c r="V89" t="s">
+        <v>160</v>
+      </c>
+      <c r="W89" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="90" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S90" t="s">
+        <v>219</v>
+      </c>
+      <c r="T90" t="s">
+        <v>158</v>
+      </c>
+      <c r="U90">
+        <v>1.9325300471382499E-2</v>
+      </c>
+      <c r="V90" t="s">
+        <v>185</v>
+      </c>
+      <c r="W90" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="91" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S91" t="s">
+        <v>164</v>
+      </c>
+      <c r="T91" t="s">
+        <v>187</v>
+      </c>
+      <c r="U91">
+        <v>1.9919086416145902E-2</v>
+      </c>
+      <c r="V91" t="s">
+        <v>165</v>
+      </c>
+      <c r="W91" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S92" t="s">
+        <v>179</v>
+      </c>
+      <c r="T92" t="s">
+        <v>171</v>
+      </c>
+      <c r="U92">
+        <v>2.0035608959591798E-2</v>
+      </c>
+      <c r="V92" t="s">
+        <v>173</v>
+      </c>
+      <c r="W92" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S93" t="s">
+        <v>171</v>
+      </c>
+      <c r="T93" t="s">
+        <v>181</v>
+      </c>
+      <c r="U93">
+        <v>2.0558817165552499E-2</v>
+      </c>
+      <c r="V93" t="s">
+        <v>167</v>
+      </c>
+      <c r="W93" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="94" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S94" t="s">
+        <v>220</v>
+      </c>
+      <c r="T94" t="s">
+        <v>158</v>
+      </c>
+      <c r="U94">
+        <v>2.055881717701E-2</v>
+      </c>
+      <c r="V94" t="s">
+        <v>185</v>
+      </c>
+      <c r="W94" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S95" t="s">
+        <v>170</v>
+      </c>
+      <c r="T95" t="s">
+        <v>180</v>
+      </c>
+      <c r="U95">
+        <v>2.1921478951254299E-2</v>
+      </c>
+      <c r="V95" t="s">
+        <v>167</v>
+      </c>
+      <c r="W95" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S96" t="s">
+        <v>186</v>
+      </c>
+      <c r="T96" t="s">
+        <v>164</v>
+      </c>
+      <c r="U96">
+        <v>2.4699634742740201E-2</v>
+      </c>
+      <c r="V96" t="s">
+        <v>183</v>
+      </c>
+      <c r="W96" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="97" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S97" t="s">
+        <v>171</v>
+      </c>
+      <c r="T97" t="s">
+        <v>180</v>
+      </c>
+      <c r="U97">
+        <v>2.5052551377114301E-2</v>
+      </c>
+      <c r="V97" t="s">
+        <v>167</v>
+      </c>
+      <c r="W97" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S98" t="s">
+        <v>221</v>
+      </c>
+      <c r="T98" t="s">
+        <v>158</v>
+      </c>
+      <c r="U98">
+        <v>2.6238702047542299E-2</v>
+      </c>
+      <c r="V98" t="s">
+        <v>185</v>
+      </c>
+      <c r="W98" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S99" t="s">
+        <v>170</v>
+      </c>
+      <c r="T99" t="s">
+        <v>153</v>
+      </c>
+      <c r="U99">
+        <v>3.1386363486935603E-2</v>
+      </c>
+      <c r="V99" t="s">
+        <v>167</v>
+      </c>
+      <c r="W99" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="100" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S100" t="s">
+        <v>171</v>
+      </c>
+      <c r="T100" t="s">
+        <v>153</v>
+      </c>
+      <c r="U100">
+        <v>3.5301633234049799E-2</v>
+      </c>
+      <c r="V100" t="s">
+        <v>167</v>
+      </c>
+      <c r="W100" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="101" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S101" t="s">
+        <v>162</v>
+      </c>
+      <c r="T101" t="s">
+        <v>206</v>
+      </c>
+      <c r="U101">
+        <v>3.5301633271287797E-2</v>
+      </c>
+      <c r="V101" t="s">
+        <v>163</v>
+      </c>
+      <c r="W101" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S102" t="s">
+        <v>162</v>
+      </c>
+      <c r="T102" t="s">
+        <v>207</v>
+      </c>
+      <c r="U102">
+        <v>3.53016332899109E-2</v>
+      </c>
+      <c r="V102" t="s">
+        <v>163</v>
+      </c>
+      <c r="W102" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S103" t="s">
+        <v>162</v>
+      </c>
+      <c r="T103" t="s">
+        <v>211</v>
+      </c>
+      <c r="U103">
+        <v>3.7417399720575603E-2</v>
+      </c>
+      <c r="V103" t="s">
+        <v>163</v>
+      </c>
+      <c r="W103" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S104" t="s">
+        <v>162</v>
+      </c>
+      <c r="T104" t="s">
+        <v>155</v>
+      </c>
+      <c r="U104">
+        <v>3.9644683838313099E-2</v>
+      </c>
+      <c r="V104" t="s">
+        <v>163</v>
+      </c>
+      <c r="W104" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S105" t="s">
+        <v>158</v>
+      </c>
+      <c r="T105" t="s">
+        <v>222</v>
+      </c>
+      <c r="U105">
+        <v>4.445279133321E-2</v>
+      </c>
+      <c r="V105" t="s">
+        <v>160</v>
+      </c>
+      <c r="W105" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="106" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S106" t="s">
+        <v>223</v>
+      </c>
+      <c r="T106" t="s">
+        <v>159</v>
+      </c>
+      <c r="U106">
+        <v>4.4452791333214899E-2</v>
+      </c>
+      <c r="V106" t="s">
+        <v>215</v>
+      </c>
+      <c r="W106" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="107" spans="19:23" x14ac:dyDescent="0.2">
+      <c r="S107" t="s">
+        <v>224</v>
+      </c>
+      <c r="T107" t="s">
+        <v>158</v>
+      </c>
+      <c r="U107">
+        <v>4.9765026710464601E-2</v>
+      </c>
+      <c r="V107" t="s">
+        <v>185</v>
+      </c>
+      <c r="W107" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8DFD34-F077-8C42-9272-0EF6BC9716AF}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1537,4 +4757,376 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD607BF-197B-2147-AC05-4F3DD22E7F57}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.67987070000000005</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.49E-22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4">
+        <v>0.40730099962976701</v>
+      </c>
+      <c r="H4">
+        <v>3.5414370771533898E-4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>247</v>
+      </c>
+      <c r="L4">
+        <v>0.24583987508593899</v>
+      </c>
+      <c r="M4">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N4">
+        <v>1.92797219198881E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.60943897999999996</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3.8500000000000003E-18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G5">
+        <v>0.33202763442327798</v>
+      </c>
+      <c r="H5">
+        <v>3.8517553155409702E-3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>248</v>
+      </c>
+      <c r="L5">
+        <v>0.170447431082971</v>
+      </c>
+      <c r="M5">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N5">
+        <v>5.2427385760590896E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.48168482000000001</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4.1200000000000002E-12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6">
+        <v>-0.244948129944738</v>
+      </c>
+      <c r="H6">
+        <v>3.5430071064763202E-2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>249</v>
+      </c>
+      <c r="L6">
+        <v>0.161177079209195</v>
+      </c>
+      <c r="M6">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N6">
+        <v>7.8731176309350601E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.46950112999999999</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.27E-11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7">
+        <v>-0.23363717822524899</v>
+      </c>
+      <c r="H7">
+        <v>4.5131533014349502E-2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>250</v>
+      </c>
+      <c r="L7">
+        <v>0.14045779554406099</v>
+      </c>
+      <c r="M7">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N7">
+        <v>1.7893927900063E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.25063133999999998</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D8" s="6">
+        <v>7.1799999999999999E-6</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.190344316919659</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0.10423534325961099</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="L8" s="9">
+        <v>1.5763568133341499E-3</v>
+      </c>
+      <c r="M8" s="9">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.41707607148472298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.27441321000000002</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2.2799999999999999E-5</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="9">
+        <v>-6.2170487537177299E-2</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.598738663095706</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="L9" s="9">
+        <v>-3.00027146041216E-2</v>
+      </c>
+      <c r="M9" s="9">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0.590842070778272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.24124828000000001</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0724E-4</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="L10" s="9">
+        <v>-5.5698022730761597E-2</v>
+      </c>
+      <c r="M10" s="9">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0.71645426212670604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.15044637999999999</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.2754699999999999E-3</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="L11" s="9">
+        <v>-5.6975599238977999E-2</v>
+      </c>
+      <c r="M11" s="9">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0.721964888477161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="9">
+        <v>-3.5106400000000003E-2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-1.36986E-2</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.61665159000000003</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="L12" s="9">
+        <v>-5.6533493498389202E-2</v>
+      </c>
+      <c r="M12" s="9">
+        <v>-1.3698630136986301E-2</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0.72590024136241604</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D12">
+    <sortCondition ref="D4:D12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>